<commit_message>
Updated 'Sheet1' via CrewAI tool
</commit_message>
<xml_diff>
--- a/Hotcard Ticket.xlsx
+++ b/Hotcard Ticket.xlsx
@@ -815,7 +815,11 @@
           <t>bins</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr"/>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">

</xml_diff>